<commit_message>
We added the fourth example
</commit_message>
<xml_diff>
--- a/Databases and Sources.xlsx
+++ b/Databases and Sources.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Country</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>SERIE: OCUPADOS POR RAMA DE ACTIVIDAD ECONÓMICA Y SEGÚN TRIMESTRE</t>
+  </si>
+  <si>
+    <t>Estimador Mensual de Actividad Económica. Números índice, base 2004=100 y variaciones porcentuales.</t>
+  </si>
+  <si>
+    <t>example_cleaning_databases_4</t>
+  </si>
+  <si>
+    <t>https://www.indec.gob.ar/indec/web/Nivel4-Tema-3-9-48</t>
   </si>
 </sst>
 </file>
@@ -390,64 +399,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="72.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
@@ -457,20 +484,20 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
+      <c r="A5" t="s">
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>